<commit_message>
fixed empty outputs? testing
</commit_message>
<xml_diff>
--- a/differences/excel/SUMMARY_vs_REPORT.xlsx
+++ b/differences/excel/SUMMARY_vs_REPORT.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Source 1</t>
   </si>
@@ -54,67 +54,10 @@
     <t># Chapter Count Differences</t>
   </si>
   <si>
-    <t>Words 1</t>
-  </si>
-  <si>
-    <t>Words 2</t>
-  </si>
-  <si>
-    <t>Word Indices 1</t>
-  </si>
-  <si>
-    <t>Word Indices 2</t>
-  </si>
-  <si>
-    <t>Chapter # 1</t>
-  </si>
-  <si>
-    <t>Chapter # 2</t>
-  </si>
-  <si>
-    <t>Letter 1</t>
-  </si>
-  <si>
-    <t>Letter 2</t>
-  </si>
-  <si>
-    <t>Word 1</t>
-  </si>
-  <si>
-    <t>Word 2</t>
-  </si>
-  <si>
-    <t>Letter Index 1</t>
-  </si>
-  <si>
-    <t>Letter Index 2</t>
-  </si>
-  <si>
-    <t>Word Index 1</t>
-  </si>
-  <si>
-    <t>Word Index 2</t>
-  </si>
-  <si>
-    <t>Name 1</t>
-  </si>
-  <si>
-    <t>Name 2</t>
-  </si>
-  <si>
-    <t>Count 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Count 2</t>
-  </si>
-  <si>
-    <t>Count 2</t>
-  </si>
-  <si>
-    <t>Chapter Index 1</t>
-  </si>
-  <si>
-    <t>Chapter Index 2</t>
+    <t>SUMMARY</t>
+  </si>
+  <si>
+    <t>REPORT</t>
   </si>
 </sst>
 </file>
@@ -472,13 +415,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:11">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,37 +453,39 @@
         <v>9</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="2:7">
-      <c r="B1" s="1" t="s">
+    <row r="2" spans="1:11">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
+      <c r="D2">
+        <v>2925</v>
+      </c>
+      <c r="E2">
+        <v>60690</v>
+      </c>
+      <c r="F2">
+        <v>312403</v>
+      </c>
+      <c r="G2">
+        <v>613577</v>
+      </c>
+      <c r="H2">
+        <v>1229</v>
+      </c>
+      <c r="I2">
+        <v>88</v>
+      </c>
+      <c r="J2">
+        <v>992</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -548,239 +493,98 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="2:11">
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="2:11">
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="2:11">
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="2:5">
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="2:5">
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="2:5">
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="2:3">
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>